<commit_message>
add email in vendor_details
</commit_message>
<xml_diff>
--- a/Vendor Profile.xlsx
+++ b/Vendor Profile.xlsx
@@ -23,19 +23,19 @@
     <t>Vendor Name:</t>
   </si>
   <si>
-    <t>2GO Express</t>
+    <t xml:space="preserve">	K-Mart</t>
   </si>
   <si>
     <t>Address:</t>
   </si>
   <si>
-    <t>BREDCO, Port 2, Reclamation Area, Brgy. 10, Bacolod City</t>
+    <t>Galo-Hilado St,. Brgy. 22, Bacolod, 6100 Negros Occidental</t>
   </si>
   <si>
     <t>Phone Number:</t>
   </si>
   <si>
-    <t>(034) 704-1339</t>
+    <t>(034) 434 6914, 434-6915</t>
   </si>
   <si>
     <t>Fax Number:</t>
@@ -469,10 +469,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -573,9 +573,25 @@
       </c>
       <c r="D10" s="4"/>
     </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A10:B10"/>

</xml_diff>